<commit_message>
Arquivo atualizado em 07/12/2023, 14:20:05.
</commit_message>
<xml_diff>
--- a/Data/g1.5.xlsx
+++ b/Data/g1.5.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -465,11 +461,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>40179</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>01/01/2010</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3287018248531148</v>
+        <v>32.87018248531147</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -483,11 +481,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>40544</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>01/01/2011</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>0.3321590756931181</v>
+        <v>33.21590756931181</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -501,11 +501,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>40909</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>01/01/2012</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>0.3379157008864418</v>
+        <v>33.79157008864419</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -519,11 +521,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>41275</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>01/01/2013</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3417742368344694</v>
+        <v>34.17742368344695</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -537,11 +541,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>41640</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>01/01/2014</t>
+        </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3461542386923597</v>
+        <v>34.61542386923598</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -555,11 +561,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>42005</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>01/01/2015</t>
+        </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3547237418540712</v>
+        <v>35.47237418540713</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -573,11 +581,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>42370</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>01/01/2016</t>
+        </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3555870740851341</v>
+        <v>35.55870740851341</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -591,11 +601,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>42736</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>01/01/2017</t>
+        </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3511293559663597</v>
+        <v>35.11293559663597</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -609,11 +621,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>43101</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>01/01/2018</t>
+        </is>
       </c>
       <c r="C10" t="n">
-        <v>0.3458379835585836</v>
+        <v>34.58379835585836</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -627,11 +641,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>43466</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>0.3437065874187381</v>
+        <v>34.37065874187381</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -645,11 +661,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>43831</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
       </c>
       <c r="C12" t="n">
-        <v>0.3327326006882678</v>
+        <v>33.27326006882678</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -663,11 +681,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>44197</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
       </c>
       <c r="C13" t="n">
-        <v>0.3101386995455688</v>
+        <v>31.01386995455688</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -681,11 +701,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B14" s="2" t="n">
-        <v>40179</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>01/01/2010</t>
+        </is>
       </c>
       <c r="C14" t="n">
-        <v>0.3607618087088878</v>
+        <v>36.07618087088878</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -699,11 +721,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>40544</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>01/01/2011</t>
+        </is>
       </c>
       <c r="C15" t="n">
-        <v>0.3683872655155243</v>
+        <v>36.83872655155243</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -717,11 +741,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B16" s="2" t="n">
-        <v>40909</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>01/01/2012</t>
+        </is>
       </c>
       <c r="C16" t="n">
-        <v>0.3685409073958112</v>
+        <v>36.85409073958112</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -735,11 +761,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B17" s="2" t="n">
-        <v>41275</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>01/01/2013</t>
+        </is>
       </c>
       <c r="C17" t="n">
-        <v>0.3754752254505626</v>
+        <v>37.54752254505625</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -753,11 +781,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B18" s="2" t="n">
-        <v>41640</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>01/01/2014</t>
+        </is>
       </c>
       <c r="C18" t="n">
-        <v>0.3774175203362666</v>
+        <v>37.74175203362666</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -771,11 +801,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B19" s="2" t="n">
-        <v>42005</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>01/01/2015</t>
+        </is>
       </c>
       <c r="C19" t="n">
-        <v>0.3818229894195735</v>
+        <v>38.18229894195735</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -789,11 +821,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B20" s="2" t="n">
-        <v>42370</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>01/01/2016</t>
+        </is>
       </c>
       <c r="C20" t="n">
-        <v>0.3771705269827347</v>
+        <v>37.71705269827347</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -807,11 +841,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B21" s="2" t="n">
-        <v>42736</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>01/01/2017</t>
+        </is>
       </c>
       <c r="C21" t="n">
-        <v>0.3707115292214108</v>
+        <v>37.07115292214107</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -825,11 +861,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B22" s="2" t="n">
-        <v>43101</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>01/01/2018</t>
+        </is>
       </c>
       <c r="C22" t="n">
-        <v>0.3691859072787141</v>
+        <v>36.91859072787141</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -843,11 +881,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B23" s="2" t="n">
-        <v>43466</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
       </c>
       <c r="C23" t="n">
-        <v>0.3684978129936551</v>
+        <v>36.84978129936551</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -861,11 +901,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B24" s="2" t="n">
-        <v>43831</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
       </c>
       <c r="C24" t="n">
-        <v>0.3487353466431323</v>
+        <v>34.87353466431323</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -879,11 +921,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B25" s="2" t="n">
-        <v>44197</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
       </c>
       <c r="C25" t="n">
-        <v>0.33225668610586</v>
+        <v>33.225668610586</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -897,11 +941,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B26" s="2" t="n">
-        <v>40179</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>01/01/2010</t>
+        </is>
       </c>
       <c r="C26" t="n">
-        <v>0.3587530585736854</v>
+        <v>35.87530585736854</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -915,11 +961,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B27" s="2" t="n">
-        <v>40544</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>01/01/2011</t>
+        </is>
       </c>
       <c r="C27" t="n">
-        <v>0.3618388015316681</v>
+        <v>36.18388015316681</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -933,11 +981,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B28" s="2" t="n">
-        <v>40909</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>01/01/2012</t>
+        </is>
       </c>
       <c r="C28" t="n">
-        <v>0.3615817811235661</v>
+        <v>36.15817811235661</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -951,11 +1001,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B29" s="2" t="n">
-        <v>41275</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>01/01/2013</t>
+        </is>
       </c>
       <c r="C29" t="n">
-        <v>0.378496745314786</v>
+        <v>37.8496745314786</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -969,11 +1021,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B30" s="2" t="n">
-        <v>41640</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>01/01/2014</t>
+        </is>
       </c>
       <c r="C30" t="n">
-        <v>0.3928978222821129</v>
+        <v>39.28978222821129</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -987,11 +1041,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B31" s="2" t="n">
-        <v>42005</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>01/01/2015</t>
+        </is>
       </c>
       <c r="C31" t="n">
-        <v>0.4010075487342685</v>
+        <v>40.10075487342684</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1005,11 +1061,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B32" s="2" t="n">
-        <v>42370</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>01/01/2016</t>
+        </is>
       </c>
       <c r="C32" t="n">
-        <v>0.390752952226525</v>
+        <v>39.0752952226525</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1023,11 +1081,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B33" s="2" t="n">
-        <v>42736</v>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>01/01/2017</t>
+        </is>
       </c>
       <c r="C33" t="n">
-        <v>0.3939763573820166</v>
+        <v>39.39763573820166</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1041,11 +1101,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B34" s="2" t="n">
-        <v>43101</v>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>01/01/2018</t>
+        </is>
       </c>
       <c r="C34" t="n">
-        <v>0.3939674645413783</v>
+        <v>39.39674645413783</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1059,11 +1121,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B35" s="2" t="n">
-        <v>43466</v>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
       </c>
       <c r="C35" t="n">
-        <v>0.3856184008937908</v>
+        <v>38.56184008937908</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1077,11 +1141,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B36" s="2" t="n">
-        <v>43831</v>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
       </c>
       <c r="C36" t="n">
-        <v>0.3721394096405206</v>
+        <v>37.21394096405206</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1095,11 +1161,13 @@
           <t>Salários</t>
         </is>
       </c>
-      <c r="B37" s="2" t="n">
-        <v>44197</v>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
       </c>
       <c r="C37" t="n">
-        <v>0.3505869720772253</v>
+        <v>35.05869720772253</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>

</xml_diff>